<commit_message>
update dei vari log di lavoro
</commit_message>
<xml_diff>
--- a/ore_progetto.xlsx
+++ b/ore_progetto.xlsx
@@ -133,7 +133,7 @@
     <t xml:space="preserve">Impostazione D2, use case </t>
   </si>
   <si>
-    <t xml:space="preserve">13/10/2022</t>
+    <t xml:space="preserve">14/10/2022</t>
   </si>
   <si>
     <t xml:space="preserve">revisione diagrammi</t>
@@ -175,7 +175,7 @@
     <t xml:space="preserve">05/11/2022</t>
   </si>
   <si>
-    <t xml:space="preserve">report per il diagramma 4</t>
+    <t xml:space="preserve">review del diagramma 4</t>
   </si>
   <si>
     <t xml:space="preserve">Sistemazione D1, D2 + diagramma componenti</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">15/11/2002</t>
   </si>
   <si>
-    <t xml:space="preserve">fine review diagramma 3 e divisione lavoro diagramma 4</t>
+    <t xml:space="preserve">fine review diagramma 3 e divisione lavoro deliverable 4</t>
   </si>
   <si>
     <t xml:space="preserve">review doc + lavoro a diagramma 4</t>
@@ -540,10 +540,10 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15:G15"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.74"/>
@@ -556,11 +556,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="4.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="11.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="11.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="4.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="22" style="0" width="11.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="12.75"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
aggiornate ore di gruppo
</commit_message>
<xml_diff>
--- a/ore_progetto.xlsx
+++ b/ore_progetto.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="49" documentId="11_B795240B6084682CA09223C34CFB1F38977FE617" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CBCF566-C747-4157-BE75-3FCD03543AAC}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="11_B795240B6084682CA09223C34CFB1F38977FE617" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF9BF89D-82EC-4723-850F-BB65960A391B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="101">
   <si>
     <t>DATA</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>user flow</t>
+  </si>
+  <si>
+    <t>aggiornamenti svilupp0</t>
   </si>
 </sst>
 </file>
@@ -720,14 +723,32 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -736,27 +757,9 @@
     <xf numFmtId="11" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -974,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T26" sqref="T26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.67578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1000,48 +1003,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="53" t="s">
+      <c r="A1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="55" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="57"/>
-      <c r="G1" s="43"/>
-      <c r="I1" s="51" t="s">
+      <c r="F1" s="49"/>
+      <c r="G1" s="46"/>
+      <c r="I1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="53" t="s">
+      <c r="J1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="43"/>
-      <c r="M1" s="52" t="s">
+      <c r="L1" s="46"/>
+      <c r="M1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="46" t="s">
+      <c r="O1" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="42" t="s">
+      <c r="P1" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="43"/>
-      <c r="S1" s="44" t="s">
+      <c r="R1" s="46"/>
+      <c r="S1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="V1" s="49" t="s">
+      <c r="V1" s="57" t="s">
         <v>6</v>
       </c>
       <c r="W1" s="29" t="s">
@@ -1056,14 +1059,14 @@
       </c>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="45"/>
+      <c r="A2" s="44"/>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1073,25 +1076,25 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="50"/>
-      <c r="J2" s="45"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="44"/>
       <c r="K2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="45"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="45"/>
+      <c r="M2" s="44"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="44"/>
       <c r="Q2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="45"/>
-      <c r="V2" s="50"/>
+      <c r="S2" s="44"/>
+      <c r="V2" s="51"/>
       <c r="W2" s="26"/>
       <c r="X2" s="4" t="s">
         <v>7</v>
@@ -1123,7 +1126,7 @@
       <c r="G3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="50"/>
+      <c r="I3" s="51"/>
       <c r="J3" s="9">
         <v>44833</v>
       </c>
@@ -1136,7 +1139,7 @@
       <c r="M3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="47"/>
+      <c r="O3" s="55"/>
       <c r="P3" s="5">
         <v>44836</v>
       </c>
@@ -1149,7 +1152,7 @@
       <c r="S3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="50"/>
+      <c r="V3" s="51"/>
       <c r="W3" s="22" t="s">
         <v>17</v>
       </c>
@@ -1183,7 +1186,7 @@
       <c r="G4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="50"/>
+      <c r="I4" s="51"/>
       <c r="J4" s="9">
         <v>44839</v>
       </c>
@@ -1196,7 +1199,7 @@
       <c r="M4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="47"/>
+      <c r="O4" s="55"/>
       <c r="P4" s="5">
         <v>44840</v>
       </c>
@@ -1209,7 +1212,7 @@
       <c r="S4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="V4" s="50"/>
+      <c r="V4" s="51"/>
       <c r="W4" s="10">
         <v>44602</v>
       </c>
@@ -1245,7 +1248,7 @@
       <c r="G5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="50"/>
+      <c r="I5" s="51"/>
       <c r="J5" s="9">
         <v>44842</v>
       </c>
@@ -1258,7 +1261,7 @@
       <c r="M5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O5" s="47"/>
+      <c r="O5" s="55"/>
       <c r="P5" s="5">
         <v>44842</v>
       </c>
@@ -1271,7 +1274,7 @@
       <c r="S5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="V5" s="50"/>
+      <c r="V5" s="51"/>
       <c r="W5" s="10">
         <v>44630</v>
       </c>
@@ -1307,7 +1310,7 @@
       <c r="G6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="50"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="10">
         <v>44843</v>
       </c>
@@ -1320,7 +1323,7 @@
       <c r="M6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="47"/>
+      <c r="O6" s="55"/>
       <c r="P6" s="5">
         <v>44843</v>
       </c>
@@ -1333,7 +1336,7 @@
       <c r="S6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="V6" s="50"/>
+      <c r="V6" s="51"/>
       <c r="W6" s="10">
         <v>44661</v>
       </c>
@@ -1369,7 +1372,7 @@
       <c r="G7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="50"/>
+      <c r="I7" s="51"/>
       <c r="J7" s="10">
         <v>44844</v>
       </c>
@@ -1382,7 +1385,7 @@
       <c r="M7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="47"/>
+      <c r="O7" s="55"/>
       <c r="P7" s="5">
         <v>44856</v>
       </c>
@@ -1396,7 +1399,7 @@
         <v>29</v>
       </c>
       <c r="T7" s="11"/>
-      <c r="V7" s="50"/>
+      <c r="V7" s="51"/>
       <c r="W7" s="10">
         <v>44840</v>
       </c>
@@ -1432,7 +1435,7 @@
       <c r="G8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="50"/>
+      <c r="I8" s="51"/>
       <c r="J8" s="10" t="s">
         <v>31</v>
       </c>
@@ -1445,7 +1448,7 @@
       <c r="M8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="47"/>
+      <c r="O8" s="55"/>
       <c r="P8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1458,7 +1461,7 @@
       <c r="S8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="V8" s="50"/>
+      <c r="V8" s="51"/>
       <c r="W8" s="21">
         <v>44841</v>
       </c>
@@ -1494,7 +1497,7 @@
       <c r="G9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="50"/>
+      <c r="I9" s="51"/>
       <c r="J9" s="10">
         <v>44854</v>
       </c>
@@ -1507,7 +1510,7 @@
       <c r="M9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="O9" s="47"/>
+      <c r="O9" s="55"/>
       <c r="P9" s="5">
         <v>44753</v>
       </c>
@@ -1520,7 +1523,7 @@
       <c r="S9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="V9" s="50"/>
+      <c r="V9" s="51"/>
       <c r="W9" s="21">
         <v>44842</v>
       </c>
@@ -1556,7 +1559,7 @@
       <c r="G10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="50"/>
+      <c r="I10" s="51"/>
       <c r="J10" s="12">
         <v>44857</v>
       </c>
@@ -1569,7 +1572,7 @@
       <c r="M10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O10" s="47"/>
+      <c r="O10" s="55"/>
       <c r="P10" s="5">
         <v>44873</v>
       </c>
@@ -1582,7 +1585,7 @@
       <c r="S10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="V10" s="50"/>
+      <c r="V10" s="51"/>
       <c r="W10" s="21">
         <v>44843</v>
       </c>
@@ -1618,7 +1621,7 @@
       <c r="G11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="50"/>
+      <c r="I11" s="51"/>
       <c r="J11" s="12">
         <v>44859</v>
       </c>
@@ -1631,7 +1634,7 @@
       <c r="M11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="O11" s="47"/>
+      <c r="O11" s="55"/>
       <c r="P11" s="5">
         <v>44885</v>
       </c>
@@ -1644,7 +1647,7 @@
       <c r="S11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="V11" s="50"/>
+      <c r="V11" s="51"/>
       <c r="W11" s="21" t="s">
         <v>45</v>
       </c>
@@ -1680,7 +1683,7 @@
       <c r="G12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="45"/>
+      <c r="I12" s="44"/>
       <c r="J12" s="9">
         <v>44870</v>
       </c>
@@ -1693,7 +1696,7 @@
       <c r="M12" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="O12" s="47"/>
+      <c r="O12" s="55"/>
       <c r="P12" s="13">
         <v>44887</v>
       </c>
@@ -1706,7 +1709,7 @@
       <c r="S12" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="V12" s="50"/>
+      <c r="V12" s="51"/>
       <c r="W12" s="21" t="s">
         <v>50</v>
       </c>
@@ -1740,7 +1743,7 @@
       <c r="G13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="51"/>
+      <c r="I13" s="50"/>
       <c r="J13" s="9">
         <v>44871</v>
       </c>
@@ -1753,7 +1756,7 @@
       <c r="M13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="O13" s="47"/>
+      <c r="O13" s="55"/>
       <c r="P13" s="16">
         <v>44888</v>
       </c>
@@ -1766,7 +1769,7 @@
       <c r="S13" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="V13" s="50"/>
+      <c r="V13" s="51"/>
       <c r="W13" s="18">
         <v>44891</v>
       </c>
@@ -1802,7 +1805,7 @@
       <c r="G14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="50"/>
+      <c r="I14" s="51"/>
       <c r="J14" s="9">
         <v>44872</v>
       </c>
@@ -1815,7 +1818,7 @@
       <c r="M14" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O14" s="47"/>
+      <c r="O14" s="55"/>
       <c r="P14" s="16">
         <v>44893</v>
       </c>
@@ -1828,7 +1831,7 @@
       <c r="S14" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="V14" s="50"/>
+      <c r="V14" s="51"/>
       <c r="W14" s="23" t="s">
         <v>59</v>
       </c>
@@ -1864,7 +1867,7 @@
       <c r="G15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="50"/>
+      <c r="I15" s="51"/>
       <c r="J15" s="9">
         <v>44881</v>
       </c>
@@ -1877,7 +1880,7 @@
       <c r="M15" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="O15" s="47"/>
+      <c r="O15" s="55"/>
       <c r="P15" s="16">
         <v>44895</v>
       </c>
@@ -1890,7 +1893,7 @@
       <c r="S15" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="V15" s="50"/>
+      <c r="V15" s="51"/>
       <c r="W15" s="21">
         <v>44872</v>
       </c>
@@ -1926,7 +1929,7 @@
       <c r="G16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="50"/>
+      <c r="I16" s="51"/>
       <c r="J16" s="9">
         <v>44882</v>
       </c>
@@ -1939,7 +1942,7 @@
       <c r="M16" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="O16" s="47"/>
+      <c r="O16" s="55"/>
       <c r="P16" s="19" t="s">
         <v>68</v>
       </c>
@@ -1952,7 +1955,7 @@
       <c r="S16" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="V16" s="50"/>
+      <c r="V16" s="51"/>
       <c r="W16" s="21">
         <v>44873</v>
       </c>
@@ -1988,7 +1991,7 @@
       <c r="G17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="50"/>
+      <c r="I17" s="51"/>
       <c r="J17" s="9">
         <v>44883</v>
       </c>
@@ -2001,7 +2004,7 @@
       <c r="M17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="O17" s="47"/>
+      <c r="O17" s="55"/>
       <c r="P17" s="16">
         <v>44902</v>
       </c>
@@ -2014,7 +2017,7 @@
       <c r="S17" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="V17" s="50"/>
+      <c r="V17" s="51"/>
       <c r="W17" s="21">
         <v>44874</v>
       </c>
@@ -2050,7 +2053,7 @@
       <c r="G18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="50"/>
+      <c r="I18" s="51"/>
       <c r="J18" s="9">
         <v>44884</v>
       </c>
@@ -2063,7 +2066,7 @@
       <c r="M18" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="O18" s="47"/>
+      <c r="O18" s="55"/>
       <c r="P18" s="16">
         <v>44904</v>
       </c>
@@ -2076,7 +2079,7 @@
       <c r="S18" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="V18" s="50"/>
+      <c r="V18" s="51"/>
       <c r="W18" s="21">
         <v>44881</v>
       </c>
@@ -2112,7 +2115,7 @@
       <c r="G19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="50"/>
+      <c r="I19" s="51"/>
       <c r="J19" s="9">
         <v>44888</v>
       </c>
@@ -2125,7 +2128,7 @@
       <c r="M19" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="O19" s="47"/>
+      <c r="O19" s="55"/>
       <c r="P19" s="16">
         <v>44907</v>
       </c>
@@ -2138,7 +2141,7 @@
       <c r="S19" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="V19" s="50"/>
+      <c r="V19" s="51"/>
       <c r="W19" s="21">
         <v>44886</v>
       </c>
@@ -2174,7 +2177,7 @@
       <c r="G20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="50"/>
+      <c r="I20" s="51"/>
       <c r="J20" s="9">
         <v>44889</v>
       </c>
@@ -2187,7 +2190,7 @@
       <c r="M20" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="O20" s="47"/>
+      <c r="O20" s="55"/>
       <c r="P20" s="16">
         <v>44911</v>
       </c>
@@ -2200,7 +2203,7 @@
       <c r="S20" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="V20" s="50"/>
+      <c r="V20" s="51"/>
       <c r="W20" s="21">
         <v>44892</v>
       </c>
@@ -2236,7 +2239,7 @@
       <c r="G21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="50"/>
+      <c r="I21" s="51"/>
       <c r="J21" s="9">
         <v>44893</v>
       </c>
@@ -2249,7 +2252,7 @@
       <c r="M21" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="O21" s="47"/>
+      <c r="O21" s="55"/>
       <c r="P21" s="16">
         <v>44914</v>
       </c>
@@ -2262,7 +2265,7 @@
       <c r="S21" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="V21" s="50"/>
+      <c r="V21" s="51"/>
       <c r="W21" s="21">
         <v>44893</v>
       </c>
@@ -2298,7 +2301,7 @@
       <c r="G22" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="50"/>
+      <c r="I22" s="51"/>
       <c r="J22" s="9">
         <v>44895</v>
       </c>
@@ -2311,7 +2314,7 @@
       <c r="M22" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="O22" s="47"/>
+      <c r="O22" s="55"/>
       <c r="P22" s="16">
         <v>44915</v>
       </c>
@@ -2324,7 +2327,7 @@
       <c r="S22" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="V22" s="50"/>
+      <c r="V22" s="51"/>
       <c r="W22" s="21">
         <v>44894</v>
       </c>
@@ -2360,7 +2363,7 @@
       <c r="G23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I23" s="50"/>
+      <c r="I23" s="51"/>
       <c r="J23" s="9">
         <v>44896</v>
       </c>
@@ -2373,7 +2376,7 @@
       <c r="M23" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="O23" s="47"/>
+      <c r="O23" s="55"/>
       <c r="P23" s="16">
         <v>44916</v>
       </c>
@@ -2386,7 +2389,7 @@
       <c r="S23" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="V23" s="50"/>
+      <c r="V23" s="51"/>
       <c r="W23" s="21">
         <v>44895</v>
       </c>
@@ -2401,14 +2404,28 @@
       </c>
     </row>
     <row r="24" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="I24" s="50"/>
+      <c r="A24" s="5">
+        <v>44922</v>
+      </c>
+      <c r="B24" s="6">
+        <v>1</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="51"/>
       <c r="J24" s="9">
         <v>44897</v>
       </c>
@@ -2421,7 +2438,7 @@
       <c r="M24" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="O24" s="47"/>
+      <c r="O24" s="55"/>
       <c r="P24" s="16">
         <v>44917</v>
       </c>
@@ -2434,7 +2451,7 @@
       <c r="S24" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="V24" s="50"/>
+      <c r="V24" s="51"/>
       <c r="W24" s="21">
         <v>44902</v>
       </c>
@@ -2456,7 +2473,7 @@
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
-      <c r="I25" s="50"/>
+      <c r="I25" s="51"/>
       <c r="J25" s="9">
         <v>44901</v>
       </c>
@@ -2469,7 +2486,7 @@
       <c r="M25" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="O25" s="47"/>
+      <c r="O25" s="55"/>
       <c r="P25" s="16">
         <v>44918</v>
       </c>
@@ -2482,7 +2499,7 @@
       <c r="S25" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="V25" s="50"/>
+      <c r="V25" s="51"/>
       <c r="W25" s="21">
         <v>44903</v>
       </c>
@@ -2504,7 +2521,7 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
-      <c r="I26" s="50"/>
+      <c r="I26" s="51"/>
       <c r="J26" s="21">
         <v>44902</v>
       </c>
@@ -2517,7 +2534,7 @@
       <c r="M26" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="O26" s="47"/>
+      <c r="O26" s="55"/>
       <c r="P26" s="16">
         <v>44919</v>
       </c>
@@ -2530,8 +2547,8 @@
       <c r="S26" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="T26" s="58"/>
-      <c r="V26" s="50"/>
+      <c r="T26" s="42"/>
+      <c r="V26" s="51"/>
       <c r="W26" s="21"/>
       <c r="X26" s="22"/>
       <c r="Y26" s="22"/>
@@ -2545,7 +2562,7 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
-      <c r="I27" s="50"/>
+      <c r="I27" s="51"/>
       <c r="J27" s="21">
         <v>44903</v>
       </c>
@@ -2558,12 +2575,12 @@
       <c r="M27" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="O27" s="47"/>
+      <c r="O27" s="55"/>
       <c r="P27" s="16"/>
       <c r="Q27" s="17"/>
       <c r="R27" s="17"/>
       <c r="S27" s="17"/>
-      <c r="V27" s="50"/>
+      <c r="V27" s="51"/>
       <c r="W27" s="21"/>
       <c r="X27" s="22"/>
       <c r="Y27" s="22"/>
@@ -2577,7 +2594,7 @@
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
-      <c r="I28" s="50"/>
+      <c r="I28" s="51"/>
       <c r="J28" s="21">
         <v>44904</v>
       </c>
@@ -2590,12 +2607,12 @@
       <c r="M28" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="O28" s="47"/>
+      <c r="O28" s="55"/>
       <c r="P28" s="16"/>
       <c r="Q28" s="17"/>
       <c r="R28" s="17"/>
       <c r="S28" s="17"/>
-      <c r="V28" s="50"/>
+      <c r="V28" s="51"/>
       <c r="W28" s="21"/>
       <c r="X28" s="22"/>
       <c r="Y28" s="22"/>
@@ -2609,7 +2626,7 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
-      <c r="I29" s="50"/>
+      <c r="I29" s="51"/>
       <c r="J29" s="21">
         <v>44905</v>
       </c>
@@ -2622,12 +2639,12 @@
       <c r="M29" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="O29" s="47"/>
+      <c r="O29" s="55"/>
       <c r="P29" s="16"/>
       <c r="Q29" s="17"/>
       <c r="R29" s="17"/>
       <c r="S29" s="17"/>
-      <c r="V29" s="50"/>
+      <c r="V29" s="51"/>
       <c r="W29" s="21"/>
       <c r="X29" s="22"/>
       <c r="Y29" s="22"/>
@@ -2641,7 +2658,7 @@
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
-      <c r="I30" s="50"/>
+      <c r="I30" s="51"/>
       <c r="J30" s="21">
         <v>44907</v>
       </c>
@@ -2654,12 +2671,12 @@
       <c r="M30" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="O30" s="47"/>
+      <c r="O30" s="55"/>
       <c r="P30" s="16"/>
       <c r="Q30" s="17"/>
       <c r="R30" s="17"/>
       <c r="S30" s="17"/>
-      <c r="V30" s="50"/>
+      <c r="V30" s="51"/>
       <c r="W30" s="21"/>
       <c r="X30" s="22"/>
       <c r="Y30" s="22"/>
@@ -2673,7 +2690,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
-      <c r="I31" s="50"/>
+      <c r="I31" s="51"/>
       <c r="J31" s="21">
         <v>44910</v>
       </c>
@@ -2686,12 +2703,12 @@
       <c r="M31" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="O31" s="47"/>
+      <c r="O31" s="55"/>
       <c r="P31" s="16"/>
       <c r="Q31" s="17"/>
       <c r="R31" s="17"/>
       <c r="S31" s="17"/>
-      <c r="V31" s="50"/>
+      <c r="V31" s="51"/>
       <c r="W31" s="21"/>
       <c r="X31" s="22"/>
       <c r="Y31" s="22"/>
@@ -2705,7 +2722,7 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
-      <c r="I32" s="50"/>
+      <c r="I32" s="51"/>
       <c r="J32" s="21">
         <v>44911</v>
       </c>
@@ -2718,12 +2735,12 @@
       <c r="M32" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="O32" s="47"/>
+      <c r="O32" s="55"/>
       <c r="P32" s="16"/>
       <c r="Q32" s="17"/>
       <c r="R32" s="17"/>
       <c r="S32" s="17"/>
-      <c r="V32" s="50"/>
+      <c r="V32" s="51"/>
       <c r="W32" s="21"/>
       <c r="X32" s="22"/>
       <c r="Y32" s="22"/>
@@ -2737,17 +2754,17 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
-      <c r="I33" s="50"/>
+      <c r="I33" s="51"/>
       <c r="J33" s="9"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
       <c r="M33" s="7"/>
-      <c r="O33" s="48"/>
+      <c r="O33" s="56"/>
       <c r="P33" s="16"/>
       <c r="Q33" s="17"/>
       <c r="R33" s="17"/>
       <c r="S33" s="17"/>
-      <c r="V33" s="50"/>
+      <c r="V33" s="51"/>
       <c r="W33" s="21">
         <v>44907</v>
       </c>
@@ -2765,14 +2782,14 @@
       <c r="A34" s="24"/>
       <c r="B34">
         <f>SUM(B3:B33)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C34">
         <f>(SUM(C3:C33)/60)</f>
         <v>5.8</v>
       </c>
-      <c r="I34" s="50"/>
-      <c r="V34" s="50"/>
+      <c r="I34" s="51"/>
+      <c r="V34" s="51"/>
       <c r="W34" s="23"/>
       <c r="X34" s="23"/>
       <c r="Y34" s="23"/>
@@ -2786,9 +2803,9 @@
       <c r="E35" s="35"/>
       <c r="F35" s="35"/>
       <c r="G35" s="35"/>
-      <c r="I35" s="50"/>
+      <c r="I35" s="51"/>
       <c r="J35" s="25"/>
-      <c r="V35" s="50"/>
+      <c r="V35" s="51"/>
       <c r="W35" s="21"/>
       <c r="X35" s="22"/>
       <c r="Y35" s="22"/>
@@ -2803,8 +2820,8 @@
       <c r="F36" s="33"/>
       <c r="G36" s="33"/>
       <c r="H36" s="35"/>
-      <c r="I36" s="50"/>
-      <c r="V36" s="50"/>
+      <c r="I36" s="51"/>
+      <c r="V36" s="51"/>
       <c r="W36" s="21"/>
       <c r="X36" s="22"/>
       <c r="Y36" s="22"/>
@@ -2819,8 +2836,8 @@
       <c r="F37" s="33"/>
       <c r="G37" s="33"/>
       <c r="H37" s="35"/>
-      <c r="I37" s="50"/>
-      <c r="V37" s="50"/>
+      <c r="I37" s="51"/>
+      <c r="V37" s="51"/>
       <c r="W37" s="21"/>
       <c r="X37" s="22"/>
       <c r="Y37" s="22"/>
@@ -2835,8 +2852,8 @@
       <c r="F38" s="33"/>
       <c r="G38" s="33"/>
       <c r="H38" s="35"/>
-      <c r="I38" s="50"/>
-      <c r="V38" s="50"/>
+      <c r="I38" s="51"/>
+      <c r="V38" s="51"/>
       <c r="W38" s="21"/>
       <c r="X38" s="22"/>
       <c r="Y38" s="22"/>
@@ -2851,8 +2868,8 @@
       <c r="F39" s="33"/>
       <c r="G39" s="33"/>
       <c r="H39" s="35"/>
-      <c r="I39" s="50"/>
-      <c r="V39" s="45"/>
+      <c r="I39" s="51"/>
+      <c r="V39" s="44"/>
       <c r="W39" s="21"/>
       <c r="X39" s="22"/>
       <c r="Y39" s="22"/>
@@ -2867,7 +2884,7 @@
       <c r="F40" s="33"/>
       <c r="G40" s="33"/>
       <c r="H40" s="35"/>
-      <c r="I40" s="50"/>
+      <c r="I40" s="51"/>
     </row>
     <row r="41" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="30"/>
@@ -2878,7 +2895,7 @@
       <c r="F41" s="33"/>
       <c r="G41" s="33"/>
       <c r="H41" s="35"/>
-      <c r="I41" s="50"/>
+      <c r="I41" s="51"/>
     </row>
     <row r="42" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="30"/>
@@ -2889,7 +2906,7 @@
       <c r="F42" s="33"/>
       <c r="G42" s="33"/>
       <c r="H42" s="35"/>
-      <c r="I42" s="50"/>
+      <c r="I42" s="51"/>
     </row>
     <row r="43" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="30"/>
@@ -2900,7 +2917,7 @@
       <c r="F43" s="33"/>
       <c r="G43" s="33"/>
       <c r="H43" s="35"/>
-      <c r="I43" s="50"/>
+      <c r="I43" s="51"/>
     </row>
     <row r="44" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="30"/>
@@ -2911,7 +2928,7 @@
       <c r="F44" s="33"/>
       <c r="G44" s="33"/>
       <c r="H44" s="35"/>
-      <c r="I44" s="45"/>
+      <c r="I44" s="44"/>
     </row>
     <row r="45" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="30"/>
@@ -2986,15 +3003,15 @@
       </c>
       <c r="J51" s="41">
         <f>SUM(K3:K44,B34,C34)+(SUM(L3:L44)/60)</f>
-        <v>83.633333333333326</v>
+        <v>84.633333333333326</v>
       </c>
       <c r="P51" s="41">
         <f>SUM(Q3:Q44,B34,C34)+(SUM(R3:R44)/60)</f>
-        <v>86.3</v>
+        <v>87.3</v>
       </c>
       <c r="W51" s="41">
         <f>SUM(X3:X44,B34,C34)+(SUM(Y3:Y44)/60)</f>
-        <v>83.3</v>
+        <v>84.3</v>
       </c>
     </row>
     <row r="52" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5936,11 +5953,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:I12"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="O1:O33"/>
@@ -5950,6 +5962,11 @@
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="P1:P2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:I12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>